<commit_message>
Getting URL from the excel sheet
</commit_message>
<xml_diff>
--- a/ExternalData/loginData.xlsx
+++ b/ExternalData/loginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3600" windowWidth="14145" xWindow="0" yWindow="2445"/>
+    <workbookView windowHeight="3690" windowWidth="14925" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:N10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>admin</t>
   </si>
@@ -34,10 +34,13 @@
     <t>rao1232</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>https://hrmsdemo.onpassive.com</t>
+  </si>
+  <si>
     <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,15 +403,18 @@
     <col min="2" max="2" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -416,10 +422,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -427,10 +433,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -444,6 +450,7 @@
     <hyperlink r:id="rId2" ref="B2"/>
     <hyperlink r:id="rId3" ref="B3"/>
     <hyperlink r:id="rId4" ref="B4"/>
+    <hyperlink r:id="rId5" ref="G1"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Testing commit on 07062021
</commit_message>
<xml_diff>
--- a/ExternalData/loginData.xlsx
+++ b/ExternalData/loginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="2955" windowWidth="15705" xWindow="0" yWindow="2445"/>
+    <workbookView windowHeight="3165" windowWidth="15540" xWindow="4320" yWindow="3105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
-  <si>
-    <t>admin</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>admin@123</t>
   </si>
@@ -37,10 +34,16 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>https://ostaffuidev.onpassive.com/login/loginPage</t>
+  </si>
+  <si>
+    <t>Admin@123</t>
+  </si>
+  <si>
+    <t>nilanjan</t>
+  </si>
+  <si>
     <t>Fail</t>
-  </si>
-  <si>
-    <t>https://ostaffuidev.onpassive.com/</t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCellId="1" sqref="A2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,43 +409,43 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ITest litners and failed test case screen capturing
</commit_message>
<xml_diff>
--- a/ExternalData/loginData.xlsx
+++ b/ExternalData/loginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3165" windowWidth="15540" xWindow="4320" yWindow="3105"/>
+    <workbookView windowHeight="3855" windowWidth="15540" xWindow="0" yWindow="1125"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="8">
   <si>
     <t>admin@123</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>https://ostaffuidev.onpassive.com/login/loginPage</t>
-  </si>
-  <si>
-    <t>Admin@123</t>
   </si>
   <si>
     <t>nilanjan</t>
@@ -397,7 +394,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCellId="1" sqref="A2 A1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,10 +406,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -450,11 +447,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B1"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B3"/>
-    <hyperlink r:id="rId4" ref="B4"/>
-    <hyperlink r:id="rId5" ref="G1"/>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink r:id="rId4" ref="G1"/>
+    <hyperlink r:id="rId5" ref="B1"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>